<commit_message>
update fire scar form
</commit_message>
<xml_diff>
--- a/FireScarSpecimenDataForm6-14-18.xlsx
+++ b/FireScarSpecimenDataForm6-14-18.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20341"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\burnr_develop\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Dropbox\burnr_develop\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6598E21B-C16D-4C61-8956-A8D4D181097B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="110" windowWidth="27800" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Specimen ID:</t>
   </si>
@@ -78,13 +79,16 @@
   </si>
   <si>
     <t>Clarity of Scar</t>
+  </si>
+  <si>
+    <t>"Beg rec" = when to begin recording</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +104,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -462,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -538,6 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,6 +643,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -666,6 +695,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -841,27 +887,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" customWidth="1"/>
-    <col min="2" max="5" width="6.3984375" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" customWidth="1"/>
-    <col min="7" max="7" width="4.3984375" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" customWidth="1"/>
+    <col min="2" max="5" width="6.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" customWidth="1"/>
+    <col min="7" max="7" width="4.36328125" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="5.86328125" customWidth="1"/>
-    <col min="11" max="11" width="5.1328125" customWidth="1"/>
-    <col min="12" max="12" width="8.3984375" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
+    <col min="11" max="11" width="5.08984375" customWidth="1"/>
+    <col min="12" max="12" width="8.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -881,7 +927,7 @@
       </c>
       <c r="L1" s="18"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -897,7 +943,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -917,7 +963,7 @@
       </c>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="10"/>
       <c r="C4" s="41"/>
@@ -931,10 +977,10 @@
       <c r="K4" s="10"/>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -952,7 +998,7 @@
       <c r="K6" s="43"/>
       <c r="L6" s="45"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -970,7 +1016,7 @@
       <c r="K7" s="46"/>
       <c r="L7" s="47"/>
     </row>
-    <row r="8" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="44" t="s">
         <v>10</v>
       </c>
@@ -988,8 +1034,8 @@
       <c r="K8" s="41"/>
       <c r="L8" s="48"/>
     </row>
-    <row r="9" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1005,7 +1051,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1019,7 +1065,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1033,7 +1079,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1041,14 +1087,15 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="I13" s="55" t="s">
+        <v>19</v>
+      </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="32" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1125,7 @@
       <c r="K15" s="50"/>
       <c r="L15" s="51"/>
     </row>
-    <row r="16" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="22">
         <v>1</v>
       </c>
@@ -1094,7 +1141,7 @@
       <c r="K16" s="53"/>
       <c r="L16" s="54"/>
     </row>
-    <row r="17" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25">
         <v>2</v>
       </c>
@@ -1110,7 +1157,7 @@
       <c r="K17" s="39"/>
       <c r="L17" s="40"/>
     </row>
-    <row r="18" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25">
         <v>3</v>
       </c>
@@ -1126,7 +1173,7 @@
       <c r="K18" s="39"/>
       <c r="L18" s="40"/>
     </row>
-    <row r="19" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="25">
         <v>4</v>
       </c>
@@ -1142,7 +1189,7 @@
       <c r="K19" s="39"/>
       <c r="L19" s="40"/>
     </row>
-    <row r="20" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25">
         <v>5</v>
       </c>
@@ -1158,7 +1205,7 @@
       <c r="K20" s="39"/>
       <c r="L20" s="40"/>
     </row>
-    <row r="21" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25">
         <v>6</v>
       </c>
@@ -1174,7 +1221,7 @@
       <c r="K21" s="39"/>
       <c r="L21" s="40"/>
     </row>
-    <row r="22" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="25">
         <v>7</v>
       </c>
@@ -1190,7 +1237,7 @@
       <c r="K22" s="39"/>
       <c r="L22" s="40"/>
     </row>
-    <row r="23" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25">
         <v>8</v>
       </c>
@@ -1206,7 +1253,7 @@
       <c r="K23" s="39"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25">
         <v>9</v>
       </c>
@@ -1222,7 +1269,7 @@
       <c r="K24" s="39"/>
       <c r="L24" s="40"/>
     </row>
-    <row r="25" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25">
         <v>10</v>
       </c>
@@ -1238,7 +1285,7 @@
       <c r="K25" s="39"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25">
         <v>11</v>
       </c>
@@ -1254,7 +1301,7 @@
       <c r="K26" s="39"/>
       <c r="L26" s="40"/>
     </row>
-    <row r="27" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25">
         <v>12</v>
       </c>
@@ -1270,7 +1317,7 @@
       <c r="K27" s="39"/>
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
         <v>13</v>
       </c>
@@ -1286,7 +1333,7 @@
       <c r="K28" s="39"/>
       <c r="L28" s="40"/>
     </row>
-    <row r="29" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="25">
         <v>14</v>
       </c>
@@ -1302,7 +1349,7 @@
       <c r="K29" s="39"/>
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="25">
         <v>15</v>
       </c>
@@ -1318,7 +1365,7 @@
       <c r="K30" s="39"/>
       <c r="L30" s="40"/>
     </row>
-    <row r="31" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="25">
         <v>16</v>
       </c>
@@ -1334,7 +1381,7 @@
       <c r="K31" s="39"/>
       <c r="L31" s="40"/>
     </row>
-    <row r="32" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25">
         <v>17</v>
       </c>
@@ -1350,7 +1397,7 @@
       <c r="K32" s="39"/>
       <c r="L32" s="40"/>
     </row>
-    <row r="33" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25">
         <v>18</v>
       </c>
@@ -1366,7 +1413,7 @@
       <c r="K33" s="39"/>
       <c r="L33" s="40"/>
     </row>
-    <row r="34" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25">
         <v>19</v>
       </c>
@@ -1382,7 +1429,7 @@
       <c r="K34" s="39"/>
       <c r="L34" s="40"/>
     </row>
-    <row r="35" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25">
         <v>20</v>
       </c>
@@ -1400,6 +1447,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H19:L19"/>
     <mergeCell ref="H33:L33"/>
     <mergeCell ref="H34:L34"/>
     <mergeCell ref="H35:L35"/>
@@ -1414,19 +1474,6 @@
     <mergeCell ref="H30:L30"/>
     <mergeCell ref="H31:L31"/>
     <mergeCell ref="H32:L32"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H19:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1437,24 +1484,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update db and data entry form
</commit_message>
<xml_diff>
--- a/FireScarSpecimenDataForm6-14-18.xlsx
+++ b/FireScarSpecimenDataForm6-14-18.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20341"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Dropbox\burnr_develop\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fire_History_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6598E21B-C16D-4C61-8956-A8D4D181097B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="110" windowWidth="27800" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="113" windowWidth="27803" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -526,6 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -549,7 +549,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,23 +642,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -695,23 +677,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -887,27 +852,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H16" sqref="H16:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" customWidth="1"/>
-    <col min="2" max="5" width="6.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" customWidth="1"/>
-    <col min="7" max="7" width="4.36328125" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" customWidth="1"/>
+    <col min="2" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.59765625" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="5.81640625" customWidth="1"/>
-    <col min="11" max="11" width="5.08984375" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" customWidth="1"/>
+    <col min="10" max="10" width="5.796875" customWidth="1"/>
+    <col min="11" max="11" width="5.06640625" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +892,7 @@
       </c>
       <c r="L1" s="18"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -943,7 +908,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -963,13 +928,13 @@
       </c>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="8"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="17"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -977,28 +942,28 @@
       <c r="K4" s="10"/>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G5" s="31"/>
     </row>
-    <row r="6" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
       <c r="G6" s="36"/>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="45"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="46"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1011,31 +976,31 @@
       <c r="H7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="47"/>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="44" t="s">
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="48"/>
+    </row>
+    <row r="8" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="17"/>
       <c r="H8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="48"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="49"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1051,7 +1016,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="13"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1065,7 +1030,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1079,7 +1044,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="15"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1087,15 +1052,16 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="I13" s="55" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="38" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="32" t="s">
         <v>11</v>
       </c>
@@ -1117,15 +1083,15 @@
       <c r="G15" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="49" t="s">
+      <c r="H15" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="51"/>
-    </row>
-    <row r="16" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52"/>
+    </row>
+    <row r="16" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="22">
         <v>1</v>
       </c>
@@ -1135,13 +1101,13 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="54"/>
-    </row>
-    <row r="17" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="55"/>
+    </row>
+    <row r="17" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="25">
         <v>2</v>
       </c>
@@ -1151,13 +1117,13 @@
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="40"/>
-    </row>
-    <row r="18" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="39"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="41"/>
+    </row>
+    <row r="18" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="25">
         <v>3</v>
       </c>
@@ -1167,13 +1133,13 @@
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
       <c r="G18" s="27"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="40"/>
-    </row>
-    <row r="19" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="41"/>
+    </row>
+    <row r="19" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="25">
         <v>4</v>
       </c>
@@ -1183,13 +1149,13 @@
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="40"/>
-    </row>
-    <row r="20" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="39"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="41"/>
+    </row>
+    <row r="20" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="25">
         <v>5</v>
       </c>
@@ -1199,13 +1165,13 @@
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
       <c r="G20" s="27"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="40"/>
-    </row>
-    <row r="21" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="39"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="41"/>
+    </row>
+    <row r="21" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="25">
         <v>6</v>
       </c>
@@ -1215,13 +1181,13 @@
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="40"/>
-    </row>
-    <row r="22" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="39"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="41"/>
+    </row>
+    <row r="22" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="25">
         <v>7</v>
       </c>
@@ -1231,13 +1197,13 @@
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="40"/>
-    </row>
-    <row r="23" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H22" s="39"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="41"/>
+    </row>
+    <row r="23" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="25">
         <v>8</v>
       </c>
@@ -1247,13 +1213,13 @@
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="40"/>
-    </row>
-    <row r="24" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="39"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="41"/>
+    </row>
+    <row r="24" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="25">
         <v>9</v>
       </c>
@@ -1263,13 +1229,13 @@
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="40"/>
-    </row>
-    <row r="25" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H24" s="39"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="41"/>
+    </row>
+    <row r="25" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="25">
         <v>10</v>
       </c>
@@ -1279,13 +1245,13 @@
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="40"/>
-    </row>
-    <row r="26" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="39"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="41"/>
+    </row>
+    <row r="26" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="25">
         <v>11</v>
       </c>
@@ -1295,13 +1261,13 @@
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="40"/>
-    </row>
-    <row r="27" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="39"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="41"/>
+    </row>
+    <row r="27" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="25">
         <v>12</v>
       </c>
@@ -1311,13 +1277,13 @@
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="40"/>
-    </row>
-    <row r="28" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="39"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="41"/>
+    </row>
+    <row r="28" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="25">
         <v>13</v>
       </c>
@@ -1327,13 +1293,13 @@
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="40"/>
-    </row>
-    <row r="29" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="41"/>
+    </row>
+    <row r="29" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="25">
         <v>14</v>
       </c>
@@ -1343,13 +1309,13 @@
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="40"/>
-    </row>
-    <row r="30" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="39"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="41"/>
+    </row>
+    <row r="30" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="25">
         <v>15</v>
       </c>
@@ -1359,13 +1325,13 @@
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="40"/>
-    </row>
-    <row r="31" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="39"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="41"/>
+    </row>
+    <row r="31" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="25">
         <v>16</v>
       </c>
@@ -1375,13 +1341,13 @@
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="40"/>
-    </row>
-    <row r="32" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H31" s="39"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="41"/>
+    </row>
+    <row r="32" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="25">
         <v>17</v>
       </c>
@@ -1391,13 +1357,13 @@
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="40"/>
-    </row>
-    <row r="33" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="39"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="41"/>
+    </row>
+    <row r="33" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="25">
         <v>18</v>
       </c>
@@ -1407,13 +1373,13 @@
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="40"/>
-    </row>
-    <row r="34" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H33" s="39"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="41"/>
+    </row>
+    <row r="34" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="25">
         <v>19</v>
       </c>
@@ -1423,13 +1389,13 @@
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="40"/>
-    </row>
-    <row r="35" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H34" s="39"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="41"/>
+    </row>
+    <row r="35" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="25">
         <v>20</v>
       </c>
@@ -1439,27 +1405,14 @@
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="40"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H19:L19"/>
     <mergeCell ref="H33:L33"/>
     <mergeCell ref="H34:L34"/>
     <mergeCell ref="H35:L35"/>
@@ -1474,6 +1427,19 @@
     <mergeCell ref="H30:L30"/>
     <mergeCell ref="H31:L31"/>
     <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H19:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1484,24 +1450,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>